<commit_message>
Fixed product name typo & adding tiny images
</commit_message>
<xml_diff>
--- a/WebDeploy/Install/Products.xlsx
+++ b/WebDeploy/Install/Products.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\ArrowTFS12\Hotcakes\HCC\Main\WebDeploy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HCC-core\WebDeploy\Install\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4776D772-4BF4-4EC6-BD3F-76EF38E549C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12720"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -220,30 +221,18 @@
     <t>$59.87</t>
   </si>
   <si>
-    <t>indiana-jones-hat.jpg</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum</t>
   </si>
   <si>
-    <t>butterfly-earings</t>
-  </si>
-  <si>
     <t>SAMPLE006</t>
   </si>
   <si>
-    <t>Butterfly Earings</t>
-  </si>
-  <si>
     <t>$29.95</t>
   </si>
   <si>
     <t>Earrings.jpg</t>
   </si>
   <si>
-    <t>Sample Butterfly Earings Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum</t>
-  </si>
-  <si>
     <t>cup-cake-sample</t>
   </si>
   <si>
@@ -410,12 +399,24 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>butterfly-earrings</t>
+  </si>
+  <si>
+    <t>Butterfly Earrings</t>
+  </si>
+  <si>
+    <t>Sample Butterfly Earrings Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum</t>
+  </si>
+  <si>
+    <t>brown-fedora-01.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -552,6 +553,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -587,6 +605,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -762,12 +797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50"/>
     <col min="2" max="3" width="8"/>
@@ -777,7 +814,7 @@
     <col min="13" max="13" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -826,7 +863,7 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -930,7 +967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1034,7 +1071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1069,10 +1106,10 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
+        <v>128</v>
+      </c>
+      <c r="M4" t="s">
         <v>65</v>
-      </c>
-      <c r="M4" t="s">
-        <v>66</v>
       </c>
       <c r="N4" t="s">
         <v>48</v>
@@ -1138,9 +1175,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -1149,10 +1186,10 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -1164,7 +1201,7 @@
         <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J5" t="s">
         <v>48</v>
@@ -1173,10 +1210,10 @@
         <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="N5" t="s">
         <v>48</v>
@@ -1242,9 +1279,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1253,10 +1290,10 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -1268,31 +1305,31 @@
         <v>46</v>
       </c>
       <c r="I6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" t="s">
         <v>76</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" t="s">
-        <v>78</v>
-      </c>
-      <c r="N6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>80</v>
       </c>
       <c r="R6" t="s">
         <v>48</v>
@@ -1346,9 +1383,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1357,22 +1394,22 @@
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J7" t="s">
         <v>48</v>
@@ -1381,16 +1418,16 @@
         <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="M7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N7" t="s">
         <v>48</v>
       </c>
       <c r="O7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P7" t="s">
         <v>48</v>
@@ -1450,9 +1487,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1461,10 +1498,10 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -1476,7 +1513,7 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s">
         <v>48</v>
@@ -1485,16 +1522,16 @@
         <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="N8" t="s">
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P8" t="s">
         <v>48</v>
@@ -1569,106 +1606,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1677,126 +1716,126 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50"/>
     <col min="2" max="2" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>104</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>109</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
         <v>110</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>111</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>113</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F5" t="s">
         <v>114</v>
       </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>117</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>118</v>
-      </c>
-      <c r="G5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F6" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1805,36 +1844,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1843,25 +1882,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the sample product images
</commit_message>
<xml_diff>
--- a/WebDeploy/Install/Products.xlsx
+++ b/WebDeploy/Install/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HCC-core\WebDeploy\Install\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4776D772-4BF4-4EC6-BD3F-76EF38E549C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA78CD0E-C4D8-4498-B35C-7761A892514C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -272,9 +272,6 @@
     <t>$1,299.00</t>
   </si>
   <si>
-    <t>Laptop.png</t>
-  </si>
-  <si>
     <t>This is a sample laptop computer. It is not for sale and is a demonstration of what products could look like in your store</t>
   </si>
   <si>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>brown-fedora-01.jpg</t>
+  </si>
+  <si>
+    <t>Laptop.jpg</t>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1106,7 +1106,7 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M4" t="s">
         <v>65</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -1189,7 +1189,7 @@
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -1213,7 +1213,7 @@
         <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N5" t="s">
         <v>48</v>
@@ -1418,16 +1418,16 @@
         <v>48</v>
       </c>
       <c r="L7" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" t="s">
         <v>82</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
         <v>83</v>
-      </c>
-      <c r="N7" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" t="s">
-        <v>84</v>
       </c>
       <c r="P7" t="s">
         <v>48</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1498,10 +1498,10 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
         <v>86</v>
-      </c>
-      <c r="E8" t="s">
-        <v>87</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -1513,25 +1513,25 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
         <v>88</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>89</v>
       </c>
-      <c r="M8" t="s">
-        <v>90</v>
-      </c>
       <c r="N8" t="s">
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P8" t="s">
         <v>48</v>
@@ -1620,10 +1620,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1631,13 +1631,13 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1645,27 +1645,27 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -1673,13 +1673,13 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
         <v>93</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -1687,27 +1687,27 @@
         <v>77</v>
       </c>
       <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
         <v>93</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>94</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1729,19 +1729,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1749,93 +1749,93 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>102</v>
-      </c>
-      <c r="F2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>105</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>106</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>107</v>
-      </c>
-      <c r="G3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
         <v>109</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>110</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>112</v>
       </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>113</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>114</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>116</v>
       </c>
-      <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>117</v>
-      </c>
-      <c r="F6" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1856,13 +1856,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1870,10 +1870,10 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
         <v>121</v>
-      </c>
-      <c r="C2" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1894,13 +1894,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed sample products cupcake typo
</commit_message>
<xml_diff>
--- a/WebDeploy/Install/Products.xlsx
+++ b/WebDeploy/Install/Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HCC-core\WebDeploy\Install\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA78CD0E-C4D8-4498-B35C-7761A892514C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115769F1-B095-4350-AC51-3026F9AF4A86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="130">
   <si>
     <t>Main</t>
   </si>
@@ -239,9 +239,6 @@
     <t>SAMPLE002</t>
   </si>
   <si>
-    <t>Cup Cake Sample</t>
-  </si>
-  <si>
     <t>$1.99</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>Savor this sweet treat from our famous collection of sample items. This product is not for sale and is a demonstration of how items could appear in your store</t>
   </si>
   <si>
-    <t>Vanilla Cup Cake with Rich Frosting</t>
-  </si>
-  <si>
     <t>cup,cake,cupcake,valentine,small,treats,baked goods</t>
   </si>
   <si>
@@ -411,6 +405,15 @@
   </si>
   <si>
     <t>Laptop.jpg</t>
+  </si>
+  <si>
+    <t>Cupcake Sample</t>
+  </si>
+  <si>
+    <t>Vanilla Cupcake with Rich Frosting</t>
+  </si>
+  <si>
+    <t>cupcake-sample</t>
   </si>
 </sst>
 </file>
@@ -800,11 +803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
     <col min="2" max="3" width="8"/>
@@ -814,7 +815,7 @@
     <col min="13" max="13" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -863,7 +864,7 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -967,7 +968,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M4" t="s">
         <v>65</v>
@@ -1175,9 +1176,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -1189,7 +1190,7 @@
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -1213,7 +1214,7 @@
         <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N5" t="s">
         <v>48</v>
@@ -1279,7 +1280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -1305,31 +1306,31 @@
         <v>46</v>
       </c>
       <c r="I6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
         <v>72</v>
       </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>73</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" t="s">
         <v>74</v>
-      </c>
-      <c r="N6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" t="s">
-        <v>75</v>
-      </c>
-      <c r="P6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>76</v>
       </c>
       <c r="R6" t="s">
         <v>48</v>
@@ -1383,9 +1384,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1394,40 +1395,40 @@
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
         <v>81</v>
-      </c>
-      <c r="J7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" t="s">
-        <v>128</v>
-      </c>
-      <c r="M7" t="s">
-        <v>82</v>
-      </c>
-      <c r="N7" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" t="s">
-        <v>83</v>
       </c>
       <c r="P7" t="s">
         <v>48</v>
@@ -1487,9 +1488,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1498,10 +1499,10 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -1513,25 +1514,25 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" t="s">
         <v>87</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" t="s">
-        <v>88</v>
-      </c>
-      <c r="M8" t="s">
-        <v>89</v>
-      </c>
       <c r="N8" t="s">
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P8" t="s">
         <v>48</v>
@@ -1609,105 +1610,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
         <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1721,121 +1722,121 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
     <col min="2" max="2" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>101</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>105</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>106</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
         <v>109</v>
       </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>111</v>
       </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>112</v>
       </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>113</v>
       </c>
-      <c r="G5" t="s">
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1849,31 +1850,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1887,20 +1888,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed remaining typos with cupcakes & manufacturers
</commit_message>
<xml_diff>
--- a/WebDeploy/Install/Products.xlsx
+++ b/WebDeploy/Install/Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HCC-core\WebDeploy\Install\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115769F1-B095-4350-AC51-3026F9AF4A86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FA2AF4-E4FF-43EE-B119-910F45F9B25C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="129">
   <si>
     <t>Main</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>Earrings.jpg</t>
-  </si>
-  <si>
-    <t>cup-cake-sample</t>
   </si>
   <si>
     <t>SAMPLE002</t>
@@ -803,7 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1107,7 +1106,7 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M4" t="s">
         <v>65</v>
@@ -1178,7 +1177,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -1190,7 +1189,7 @@
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
@@ -1214,7 +1213,7 @@
         <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N5" t="s">
         <v>48</v>
@@ -1282,7 +1281,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1291,10 +1290,10 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -1306,31 +1305,31 @@
         <v>46</v>
       </c>
       <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
         <v>71</v>
       </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>72</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6" t="s">
         <v>73</v>
-      </c>
-      <c r="N6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" t="s">
-        <v>128</v>
-      </c>
-      <c r="P6" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>74</v>
       </c>
       <c r="R6" t="s">
         <v>48</v>
@@ -1386,7 +1385,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1395,40 +1394,40 @@
         <v>42</v>
       </c>
       <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
         <v>76</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
         <v>46</v>
       </c>
       <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" t="s">
         <v>79</v>
       </c>
-      <c r="J7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" t="s">
-        <v>126</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s">
         <v>80</v>
-      </c>
-      <c r="N7" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" t="s">
-        <v>81</v>
       </c>
       <c r="P7" t="s">
         <v>48</v>
@@ -1490,7 +1489,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1499,10 +1498,10 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
         <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -1514,25 +1513,25 @@
         <v>46</v>
       </c>
       <c r="I8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
         <v>85</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>86</v>
       </c>
-      <c r="M8" t="s">
-        <v>87</v>
-      </c>
       <c r="N8" t="s">
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P8" t="s">
         <v>48</v>
@@ -1610,21 +1609,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,13 +1634,13 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,69 +1648,69 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>91</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1730,113 +1732,113 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
         <v>101</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>103</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>104</v>
-      </c>
-      <c r="G3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
         <v>106</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>109</v>
       </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>110</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
         <v>113</v>
       </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>114</v>
-      </c>
-      <c r="F6" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1857,13 +1859,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,10 +1873,10 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
         <v>118</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1895,13 +1897,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>